<commit_message>
Changed input to config
</commit_message>
<xml_diff>
--- a/blastdb/flanking_regions.xlsx
+++ b/blastdb/flanking_regions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sradak/Library/Caches/com.binarynights.ForkLift/FileCache/4F64449D-AFFD-41F3-9EB1-90BEB324E848/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sradak/Downloads/variable_extract/blastdb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C884B511-0F15-9F40-8A38-B342ACCB4236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA2B919-A468-9344-90D1-EA51687B9D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19260" xr2:uid="{D0C1844A-0301-C241-837A-D904870A691A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{D0C1844A-0301-C241-837A-D904870A691A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>CAAAAGTGGGCAGCA</t>
+  </si>
+  <si>
+    <t>Sampled Residues</t>
+  </si>
+  <si>
+    <t>APR:FED:SK:KED</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>IS::SRT:VN</t>
   </si>
 </sst>
 </file>
@@ -452,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAB6C40-4C96-8C45-B281-25BF0FCB6B5C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +488,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -493,8 +508,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -510,8 +528,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -526,6 +547,9 @@
       </c>
       <c r="E4" t="s">
         <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>